<commit_message>
Revised HG Mathers SEL to catch_quality of 2 (has ctach data to 2016 and previously assigned score of 0)
</commit_message>
<xml_diff>
--- a/data-quality/data/catch-quality_2024-09-04.xlsx
+++ b/data-quality/data/catch-quality_2024-09-04.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephaniepeacock/Salmon Watersheds Dropbox/Stephanie Peacock/X Drive/1_PROJECTS/1_Active/Population Methods and Analysis/population-indicators/data-quality/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AFAC37-081F-4041-A106-8BBA0F2B28FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7042DAD-23C6-E944-8956-0BCB80BAC065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="700" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2044" uniqueCount="466">
   <si>
     <t>region</t>
   </si>
@@ -1434,6 +1434,9 @@
   </si>
   <si>
     <t>Higher catch quality scores based on PSC-privided Fraser Catch and StockID quality.xlsx</t>
+  </si>
+  <si>
+    <t>Revised to match other HG SEL</t>
   </si>
 </sst>
 </file>
@@ -2320,8 +2323,8 @@
   <dimension ref="A1:K467"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A421" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H242" sqref="H242"/>
+      <pane ySplit="1" topLeftCell="A372" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H377" sqref="H377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13377,31 +13380,34 @@
       </c>
     </row>
     <row r="376" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A376" t="s">
+      <c r="A376" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B376" t="s">
-        <v>11</v>
-      </c>
-      <c r="C376" t="s">
+      <c r="B376" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C376" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="D376">
+      <c r="D376" s="2">
         <v>824</v>
       </c>
-      <c r="E376">
-        <v>0</v>
-      </c>
-      <c r="F376">
+      <c r="E376" s="2">
+        <v>0</v>
+      </c>
+      <c r="F376" s="2">
         <v>2016</v>
       </c>
-      <c r="G376">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="J376">
+      <c r="G376" s="2">
+        <v>2</v>
+      </c>
+      <c r="H376" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="I376" s="2"/>
+      <c r="J376" s="2">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="377" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>